<commit_message>
Created a leapMotion simulator. Need to fix a bug with ExpanDialStickCollision around the border of forearm collider (pins moving while they should not).
</commit_message>
<xml_diff>
--- a/study2-sequence.xlsx
+++ b/study2-sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.daniel\workspace\ExpanDialSticks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C2421E-7D4C-4DA7-BA9D-0D7CAFF78830}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC647E8C-6F83-4135-86FC-318FF15F807A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{60E3E7D7-20DE-4CFA-ABFC-F97E51E39363}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="9">
   <si>
     <t>Participant</t>
   </si>
@@ -50,16 +50,16 @@
     <t>Session 4</t>
   </si>
   <si>
-    <t>EDGE</t>
+    <t>SYS_OVER|USER_INT</t>
   </si>
   <si>
-    <t>SURFACE</t>
+    <t>USER_OVER|USER_INT</t>
   </si>
   <si>
-    <t>HULL</t>
+    <t>USER_OVER|SYS_INT</t>
   </si>
   <si>
-    <t>ZONE</t>
+    <t>SYS_OVER|SYS_INT</t>
   </si>
 </sst>
 </file>
@@ -88,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +122,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,19 +162,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,28 +491,28 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="1" max="5" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -503,16 +520,16 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -520,269 +537,397 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>6</v>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>2</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>3</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>5</v>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>2</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
-        <v>3</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>0</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>2</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>3</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Improving Empatica E4 control scene
</commit_message>
<xml_diff>
--- a/study2-sequence.xlsx
+++ b/study2-sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.daniel\workspace\ExpanDialSticks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC647E8C-6F83-4135-86FC-318FF15F807A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093E67DE-8575-47D4-8D71-5DB718FC31D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{60E3E7D7-20DE-4CFA-ABFC-F97E51E39363}"/>
   </bookViews>
@@ -50,16 +50,16 @@
     <t>Session 4</t>
   </si>
   <si>
-    <t>SYS_OVER|USER_INT</t>
+    <t>USERO-USERI</t>
   </si>
   <si>
-    <t>USER_OVER|USER_INT</t>
+    <t>SYSO-USERI</t>
   </si>
   <si>
-    <t>USER_OVER|SYS_INT</t>
+    <t>USERO-SYSI</t>
   </si>
   <si>
-    <t>SYS_OVER|SYS_INT</t>
+    <t>SYSO-SYSI</t>
   </si>
 </sst>
 </file>
@@ -491,12 +491,12 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="30.77734375" customWidth="1"/>
+    <col min="1" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -521,10 +521,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
@@ -544,10 +544,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -555,10 +555,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -578,10 +578,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -589,10 +589,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -612,10 +612,10 @@
         <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -623,10 +623,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>8</v>
@@ -646,10 +646,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -657,10 +657,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -680,10 +680,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -691,10 +691,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -714,10 +714,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -725,10 +725,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>7</v>
@@ -748,10 +748,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -759,10 +759,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>8</v>
@@ -782,10 +782,10 @@
         <v>8</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -793,10 +793,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>7</v>
@@ -816,10 +816,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -827,10 +827,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>8</v>
@@ -850,10 +850,10 @@
         <v>7</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -861,10 +861,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>7</v>
@@ -884,10 +884,10 @@
         <v>7</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -895,10 +895,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>8</v>
@@ -918,10 +918,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>